<commit_message>
Updated validation to find all errors before returning.
</commit_message>
<xml_diff>
--- a/test/support/fixtures/xlsx/invalid_missing_data.xlsx
+++ b/test/support/fixtures/xlsx/invalid_missing_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmaddox/code/arrow/test/support/fixtures/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1DC385A-AF31-064F-BF38-D2633EB0C486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA33601A-1046-F246-8B88-7B520D0E353D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="980" windowWidth="30240" windowHeight="17180" xr2:uid="{89E0CC38-388B-4A33-B61B-82A90C1A9AB8}"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="30240" windowHeight="17180" activeTab="1" xr2:uid="{89E0CC38-388B-4A33-B61B-82A90C1A9AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Direction 0 STOPS" sheetId="2" r:id="rId1"/>
@@ -468,7 +468,7 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -557,8 +557,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,17 +583,13 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>5271</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>5072</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -624,15 +620,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAB132A750142542B3926DCF31A13A3D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="efe259cd95b139b8a430fcab0a53d8ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0db2d361-8471-4f04-ae28-f5b2bb432068" xmlns:ns3="9ac8c65e-24cc-4907-9a10-66b1170b57fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="443ac76d90ee1648d07c0937ebde1acd" ns2:_="" ns3:_="">
     <xsd:import namespace="0db2d361-8471-4f04-ae28-f5b2bb432068"/>
@@ -861,6 +848,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C457723D-4526-420E-9AFF-DF32F9694D3B}">
   <ds:schemaRefs>
@@ -873,14 +869,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{230200EC-77C1-4FD2-9CAB-0EDB6EEE0881}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -897,4 +885,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
polish: Show all upload errors (#1079)
* Code improvements to definition uploads.

* Updated validation to find all errors before returning.
</commit_message>
<xml_diff>
--- a/test/support/fixtures/xlsx/invalid_missing_data.xlsx
+++ b/test/support/fixtures/xlsx/invalid_missing_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmaddox/code/arrow/test/support/fixtures/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1DC385A-AF31-064F-BF38-D2633EB0C486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA33601A-1046-F246-8B88-7B520D0E353D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="980" windowWidth="30240" windowHeight="17180" xr2:uid="{89E0CC38-388B-4A33-B61B-82A90C1A9AB8}"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="30240" windowHeight="17180" activeTab="1" xr2:uid="{89E0CC38-388B-4A33-B61B-82A90C1A9AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Direction 0 STOPS" sheetId="2" r:id="rId1"/>
@@ -468,7 +468,7 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -557,8 +557,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,17 +583,13 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>5271</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>5072</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -624,15 +620,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAB132A750142542B3926DCF31A13A3D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="efe259cd95b139b8a430fcab0a53d8ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0db2d361-8471-4f04-ae28-f5b2bb432068" xmlns:ns3="9ac8c65e-24cc-4907-9a10-66b1170b57fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="443ac76d90ee1648d07c0937ebde1acd" ns2:_="" ns3:_="">
     <xsd:import namespace="0db2d361-8471-4f04-ae28-f5b2bb432068"/>
@@ -861,6 +848,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C457723D-4526-420E-9AFF-DF32F9694D3B}">
   <ds:schemaRefs>
@@ -873,14 +869,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{230200EC-77C1-4FD2-9CAB-0EDB6EEE0881}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -897,4 +885,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>